<commit_message>
Actualización del proyecto para Render
</commit_message>
<xml_diff>
--- a/conversacion.xlsx
+++ b/conversacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,6 +712,58 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-09-23 11:29:21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-09-23 11:33:11</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-09-23 11:33:15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Asistente</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">¡Hola! Soy Seraphina, tu asistente de bienestar integral. ¿En qué área de tu bienestar te gustaría enfocarte hoy?
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>